<commit_message>
leetcode 341 22 93
</commit_message>
<xml_diff>
--- a/java/java_reference/src/leetcode/leetcode_summary.xlsx
+++ b/java/java_reference/src/leetcode/leetcode_summary.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaofei/repo/en-route/java/java_reference/src/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6A79A2-B812-BD49-BDEE-C84C755FA3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8A3F33-585E-714F-BFC7-BB94C319ABB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="1360" windowWidth="28040" windowHeight="17440" xr2:uid="{38E26FC4-3B33-3442-8F28-447C9CCBA886}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="33480" windowHeight="18780" xr2:uid="{38E26FC4-3B33-3442-8F28-447C9CCBA886}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
     <sheet name="说明" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">summary!$B$1:$B$234</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="264">
   <si>
     <t>Leetcode面试高频题分类刷题总结</t>
   </si>
@@ -804,6 +807,30 @@
   </si>
   <si>
     <t>子类别</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>否</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>再次深入理解并应用DFS</t>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>有思路，但边界处理不佳</t>
+  </si>
+  <si>
+    <t>递归到底，回溯保存路径</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1249,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E336D0-20F2-D048-B68A-DF908DD0420E}">
-  <dimension ref="A1:G234"/>
+  <dimension ref="A1:H234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H138" sqref="H138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -1236,10 +1264,12 @@
     <col min="4" max="4" width="78.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="24.5" style="5" customWidth="1"/>
     <col min="6" max="6" width="23.83203125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="10.83203125" style="5"/>
+    <col min="8" max="8" width="58.6640625" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -1261,8 +1291,11 @@
       <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>148</v>
       </c>
@@ -1274,7 +1307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>56</v>
       </c>
@@ -1286,7 +1319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>27</v>
       </c>
@@ -1298,7 +1331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>179</v>
       </c>
@@ -1310,7 +1343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>75</v>
       </c>
@@ -1322,7 +1355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>215</v>
       </c>
@@ -1334,7 +1367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -1346,7 +1379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>206</v>
       </c>
@@ -1358,7 +1391,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>876</v>
       </c>
@@ -1370,7 +1403,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>160</v>
       </c>
@@ -1382,7 +1415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>141</v>
       </c>
@@ -1394,7 +1427,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>92</v>
       </c>
@@ -1406,7 +1439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>328</v>
       </c>
@@ -1418,7 +1451,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>225</v>
       </c>
@@ -1429,7 +1462,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>346</v>
       </c>
@@ -2672,7 +2705,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="8">
         <v>108</v>
       </c>
@@ -2683,7 +2716,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="8">
         <v>333</v>
       </c>
@@ -2694,7 +2727,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="8">
         <v>285</v>
       </c>
@@ -2705,7 +2738,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="8">
         <v>341</v>
       </c>
@@ -2715,8 +2748,20 @@
       <c r="D132" s="9" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H132" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="8">
         <v>394</v>
       </c>
@@ -2727,7 +2772,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="8">
         <v>51</v>
       </c>
@@ -2738,7 +2783,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="8">
         <v>291</v>
       </c>
@@ -2749,7 +2794,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="8">
         <v>126</v>
       </c>
@@ -2760,7 +2805,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="8">
         <v>93</v>
       </c>
@@ -2770,8 +2815,17 @@
       <c r="D137" s="9" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E137" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G137" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H137" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="8">
         <v>22</v>
       </c>
@@ -2781,8 +2835,17 @@
       <c r="D138" s="9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E138" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G138" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H138" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="8">
         <v>856</v>
       </c>
@@ -2793,7 +2856,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="8">
         <v>301</v>
       </c>
@@ -2804,7 +2867,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="8">
         <v>37</v>
       </c>
@@ -2815,7 +2878,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="8">
         <v>212</v>
       </c>
@@ -2826,7 +2889,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="8">
         <v>1087</v>
       </c>
@@ -2837,7 +2900,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="8">
         <v>399</v>
       </c>
@@ -3856,6 +3919,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B234" xr:uid="{06E336D0-20F2-D048-B68A-DF908DD0420E}"/>
   <hyperlinks>
     <hyperlink ref="D159" r:id="rId1" display="https://link.zhihu.com/?target=https%3A//leetcode.com/explore/item/3950" xr:uid="{7958C2EB-402B-E448-9391-F3B838C883E3}"/>
     <hyperlink ref="D229" r:id="rId2" display="https://link.zhihu.com/?target=https%3A//leetcode.com/problems/wildcard-matching" xr:uid="{F4977E39-20C5-4D4A-A348-42A5D048932E}"/>

</xml_diff>

<commit_message>
leetcode 162 1472 128 20
</commit_message>
<xml_diff>
--- a/java/java_reference/src/leetcode/leetcode_summary.xlsx
+++ b/java/java_reference/src/leetcode/leetcode_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaofei/repo/en-route/java/java_reference/src/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653039B7-737E-B142-BF46-EDBFA5F9ACC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D4D3E9-9D84-A54C-9ABE-A92075E04DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="500" windowWidth="33480" windowHeight="18780" xr2:uid="{38E26FC4-3B33-3442-8F28-447C9CCBA886}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="271">
   <si>
     <t>Leetcode面试高频题分类刷题总结</t>
   </si>
@@ -840,6 +840,18 @@
   </si>
   <si>
     <t>边界情况没处理好</t>
+  </si>
+  <si>
+    <t>对dp和dfs实现有典型代表意义</t>
+  </si>
+  <si>
+    <t>基于hashmap仍然不够，还有精巧之处</t>
+  </si>
+  <si>
+    <t>边界处理比较麻烦</t>
+  </si>
+  <si>
+    <t>这个题理解起来有些问题</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1273,8 @@
   <dimension ref="A1:H234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H124" sqref="H124"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -1482,7 +1494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>281</v>
       </c>
@@ -1493,7 +1505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>1429</v>
       </c>
@@ -1504,7 +1516,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="8">
         <v>54</v>
       </c>
@@ -1515,7 +1527,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>362</v>
       </c>
@@ -1526,7 +1538,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>155</v>
       </c>
@@ -1537,7 +1549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>232</v>
       </c>
@@ -1548,7 +1560,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>150</v>
       </c>
@@ -1559,7 +1571,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>224</v>
       </c>
@@ -1570,7 +1582,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>20</v>
       </c>
@@ -1581,7 +1593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>1472</v>
       </c>
@@ -1591,8 +1603,17 @@
       <c r="D26" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>1209</v>
       </c>
@@ -1603,7 +1624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>1249</v>
       </c>
@@ -1614,7 +1635,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>735</v>
       </c>
@@ -1625,7 +1646,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>1</v>
       </c>
@@ -1636,7 +1657,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>146</v>
       </c>
@@ -1647,7 +1668,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>128</v>
       </c>
@@ -1656,6 +1677,15 @@
       </c>
       <c r="D32" s="9" t="s">
         <v>42</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1834,7 +1864,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>1438</v>
       </c>
@@ -1845,7 +1875,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>895</v>
       </c>
@@ -1856,7 +1886,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>34</v>
       </c>
@@ -1867,7 +1897,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>33</v>
       </c>
@@ -1878,7 +1908,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>1095</v>
       </c>
@@ -1889,7 +1919,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>162</v>
       </c>
@@ -1899,8 +1929,20 @@
       <c r="D54" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="8">
         <v>278</v>
       </c>
@@ -1911,7 +1953,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>74</v>
       </c>
@@ -1922,7 +1964,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>240</v>
       </c>
@@ -1933,7 +1975,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>69</v>
       </c>
@@ -1944,7 +1986,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>540</v>
       </c>
@@ -1955,7 +1997,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>644</v>
       </c>
@@ -1966,7 +2008,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="8">
         <v>528</v>
       </c>
@@ -1977,7 +2019,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>1300</v>
       </c>
@@ -1988,7 +2030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>1060</v>
       </c>
@@ -1999,7 +2041,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>1062</v>
       </c>
@@ -3114,6 +3156,15 @@
       </c>
       <c r="D158" s="9" t="s">
         <v>173</v>
+      </c>
+      <c r="E158" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G158" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H158" s="5" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>